<commit_message>
Fix to spreadsheet puzzle count
</commit_message>
<xml_diff>
--- a/50_puzzles_result.xlsx
+++ b/50_puzzles_result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,7 +449,7 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Path Length</t>
+          <t>Run Time</t>
         </is>
       </c>
     </row>
@@ -468,18 +468,18 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>286</v>
       </c>
       <c r="F2" t="n">
-        <v>0.00299382209777832</v>
+        <v>0.2240033149719238</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -490,18 +490,18 @@
         <v>1</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>184</v>
       </c>
       <c r="F3" t="n">
-        <v>0.005029201507568359</v>
+        <v>0.1329855918884277</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -512,18 +512,18 @@
         <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>251</v>
       </c>
       <c r="F4" t="n">
-        <v>0.002036094665527344</v>
+        <v>0.2160248756408691</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -534,18 +534,18 @@
         <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E5" t="n">
-        <v>7</v>
+        <v>130</v>
       </c>
       <c r="F5" t="n">
-        <v>0.002038240432739258</v>
+        <v>0.1239974498748779</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -556,18 +556,18 @@
         <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>171</v>
       </c>
       <c r="F6" t="n">
-        <v>0.005039691925048828</v>
+        <v>0.117988109588623</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -578,18 +578,18 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F7" t="n">
-        <v>0.00299525260925293</v>
+        <v>0.01198911666870117</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -600,18 +600,18 @@
         <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E8" t="n">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="F8" t="n">
-        <v>0.001996517181396484</v>
+        <v>0.02399539947509766</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -622,18 +622,18 @@
         <v>3</v>
       </c>
       <c r="D9" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F9" t="n">
-        <v>0.005031824111938477</v>
+        <v>0.009990215301513672</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -644,18 +644,18 @@
         <v>4</v>
       </c>
       <c r="D10" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E10" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="F10" t="n">
-        <v>0.003035068511962891</v>
+        <v>0.01405882835388184</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -668,18 +668,18 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E11" t="n">
-        <v>2079</v>
+        <v>736</v>
       </c>
       <c r="F11" t="n">
-        <v>26.57204127311707</v>
+        <v>1.422996282577515</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -690,18 +690,18 @@
         <v>1</v>
       </c>
       <c r="D12" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E12" t="n">
-        <v>368</v>
+        <v>397</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5880374908447266</v>
+        <v>0.6589710712432861</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -712,18 +712,18 @@
         <v>2</v>
       </c>
       <c r="D13" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E13" t="n">
-        <v>790</v>
+        <v>428</v>
       </c>
       <c r="F13" t="n">
-        <v>3.368710041046143</v>
+        <v>0.7860367298126221</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -734,18 +734,18 @@
         <v>3</v>
       </c>
       <c r="D14" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E14" t="n">
-        <v>248</v>
+        <v>203</v>
       </c>
       <c r="F14" t="n">
-        <v>0.3559553623199463</v>
+        <v>0.2419888973236084</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -756,18 +756,18 @@
         <v>4</v>
       </c>
       <c r="D15" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E15" t="n">
-        <v>360</v>
+        <v>389</v>
       </c>
       <c r="F15" t="n">
-        <v>0.7710413932800293</v>
+        <v>0.6329941749572754</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -778,18 +778,18 @@
         <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E16" t="n">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1029868125915527</v>
+        <v>0.0260012149810791</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -800,18 +800,18 @@
         <v>2</v>
       </c>
       <c r="D17" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E17" t="n">
-        <v>3048</v>
+        <v>25</v>
       </c>
       <c r="F17" t="n">
-        <v>170.5168688297272</v>
+        <v>0.01803398132324219</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -822,18 +822,18 @@
         <v>3</v>
       </c>
       <c r="D18" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E18" t="n">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="F18" t="n">
-        <v>0.1457440853118896</v>
+        <v>0.0230410099029541</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -844,18 +844,18 @@
         <v>4</v>
       </c>
       <c r="D19" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E19" t="n">
-        <v>85</v>
+        <v>21</v>
       </c>
       <c r="F19" t="n">
-        <v>0.2435760498046875</v>
+        <v>0.0149993896484375</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -868,18 +868,18 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E20" t="n">
-        <v>5309</v>
+        <v>246</v>
       </c>
       <c r="F20" t="n">
-        <v>112.2345345020294</v>
+        <v>0.1779863834381104</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -890,18 +890,18 @@
         <v>1</v>
       </c>
       <c r="D21" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E21" t="n">
-        <v>4329</v>
+        <v>157</v>
       </c>
       <c r="F21" t="n">
-        <v>63.24988555908203</v>
+        <v>0.0919651985168457</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -912,18 +912,18 @@
         <v>2</v>
       </c>
       <c r="D22" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E22" t="n">
-        <v>4245</v>
+        <v>178</v>
       </c>
       <c r="F22" t="n">
-        <v>60.7760157585144</v>
+        <v>0.1279988288879395</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -934,18 +934,18 @@
         <v>3</v>
       </c>
       <c r="D23" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E23" t="n">
-        <v>3874</v>
+        <v>151</v>
       </c>
       <c r="F23" t="n">
-        <v>50.83819198608398</v>
+        <v>0.09299373626708984</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -956,18 +956,18 @@
         <v>4</v>
       </c>
       <c r="D24" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E24" t="n">
-        <v>3731</v>
+        <v>152</v>
       </c>
       <c r="F24" t="n">
-        <v>39.93767023086548</v>
+        <v>0.08903145790100098</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -978,18 +978,18 @@
         <v>1</v>
       </c>
       <c r="D25" t="n">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="E25" t="n">
-        <v>1066</v>
+        <v>71</v>
       </c>
       <c r="F25" t="n">
-        <v>4.160038948059082</v>
+        <v>0.03003764152526855</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1000,18 +1000,18 @@
         <v>2</v>
       </c>
       <c r="D26" t="n">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="E26" t="n">
-        <v>1217</v>
+        <v>82</v>
       </c>
       <c r="F26" t="n">
-        <v>6.046000242233276</v>
+        <v>0.03300333023071289</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1022,18 +1022,18 @@
         <v>3</v>
       </c>
       <c r="D27" t="n">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="E27" t="n">
-        <v>1066</v>
+        <v>71</v>
       </c>
       <c r="F27" t="n">
-        <v>4.220002174377441</v>
+        <v>0.03700828552246094</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1044,18 +1044,18 @@
         <v>4</v>
       </c>
       <c r="D28" t="n">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="E28" t="n">
-        <v>1166</v>
+        <v>74</v>
       </c>
       <c r="F28" t="n">
-        <v>5.325945138931274</v>
+        <v>0.04003620147705078</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1067,21 +1067,19 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D29" t="n">
+        <v>9</v>
       </c>
       <c r="E29" t="n">
-        <v>156</v>
+        <v>2552</v>
       </c>
       <c r="F29" t="n">
-        <v>0.08903098106384277</v>
+        <v>18.49196171760559</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1091,21 +1089,19 @@
       <c r="C30" t="n">
         <v>1</v>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D30" t="n">
+        <v>9</v>
       </c>
       <c r="E30" t="n">
-        <v>156</v>
+        <v>1206</v>
       </c>
       <c r="F30" t="n">
-        <v>0.08600711822509766</v>
+        <v>5.473022222518921</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1115,21 +1111,19 @@
       <c r="C31" t="n">
         <v>2</v>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D31" t="n">
+        <v>9</v>
       </c>
       <c r="E31" t="n">
-        <v>156</v>
+        <v>1513</v>
       </c>
       <c r="F31" t="n">
-        <v>0.08900189399719238</v>
+        <v>7.963034629821777</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1139,21 +1133,19 @@
       <c r="C32" t="n">
         <v>3</v>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D32" t="n">
+        <v>9</v>
       </c>
       <c r="E32" t="n">
-        <v>156</v>
+        <v>669</v>
       </c>
       <c r="F32" t="n">
-        <v>0.08301758766174316</v>
+        <v>2.217032670974731</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1163,21 +1155,19 @@
       <c r="C33" t="n">
         <v>4</v>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D33" t="n">
+        <v>9</v>
       </c>
       <c r="E33" t="n">
-        <v>156</v>
+        <v>1165</v>
       </c>
       <c r="F33" t="n">
-        <v>0.08804130554199219</v>
+        <v>5.524951219558716</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1187,21 +1177,19 @@
       <c r="C34" t="n">
         <v>1</v>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D34" t="n">
+        <v>9</v>
       </c>
       <c r="E34" t="n">
-        <v>156</v>
+        <v>35</v>
       </c>
       <c r="F34" t="n">
-        <v>0.08503627777099609</v>
+        <v>0.0429990291595459</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1211,45 +1199,41 @@
       <c r="C35" t="n">
         <v>2</v>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D35" t="n">
+        <v>13</v>
       </c>
       <c r="E35" t="n">
-        <v>156</v>
+        <v>84</v>
       </c>
       <c r="F35" t="n">
-        <v>0.08801078796386719</v>
+        <v>0.2020695209503174</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
+        <v>4</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>GBFS</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>3</v>
+      </c>
+      <c r="D36" t="n">
+        <v>9</v>
+      </c>
+      <c r="E36" t="n">
         <v>35</v>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>GBFS</t>
-        </is>
-      </c>
-      <c r="C36" t="n">
-        <v>3</v>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E36" t="n">
-        <v>156</v>
-      </c>
       <c r="F36" t="n">
-        <v>0.08702969551086426</v>
+        <v>0.04423403739929199</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1259,21 +1243,19 @@
       <c r="C37" t="n">
         <v>4</v>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D37" t="n">
+        <v>12</v>
       </c>
       <c r="E37" t="n">
-        <v>156</v>
+        <v>34</v>
       </c>
       <c r="F37" t="n">
-        <v>0.09001016616821289</v>
+        <v>0.1520001888275146</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1285,21 +1267,19 @@
           <t>N/A</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D38" t="n">
+        <v>5</v>
       </c>
       <c r="E38" t="n">
-        <v>353</v>
+        <v>59</v>
       </c>
       <c r="F38" t="n">
-        <v>0.2419841289520264</v>
+        <v>0.03000378608703613</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1309,21 +1289,19 @@
       <c r="C39" t="n">
         <v>1</v>
       </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D39" t="n">
+        <v>5</v>
       </c>
       <c r="E39" t="n">
-        <v>353</v>
+        <v>51</v>
       </c>
       <c r="F39" t="n">
-        <v>0.3099560737609863</v>
+        <v>0.03101778030395508</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1333,21 +1311,19 @@
       <c r="C40" t="n">
         <v>2</v>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D40" t="n">
+        <v>5</v>
       </c>
       <c r="E40" t="n">
-        <v>353</v>
+        <v>56</v>
       </c>
       <c r="F40" t="n">
-        <v>0.2439785003662109</v>
+        <v>0.02999639511108398</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1357,21 +1333,19 @@
       <c r="C41" t="n">
         <v>3</v>
       </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D41" t="n">
+        <v>5</v>
       </c>
       <c r="E41" t="n">
-        <v>353</v>
+        <v>48</v>
       </c>
       <c r="F41" t="n">
-        <v>0.2927815914154053</v>
+        <v>0.02102851867675781</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -1381,21 +1355,19 @@
       <c r="C42" t="n">
         <v>4</v>
       </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D42" t="n">
+        <v>5</v>
       </c>
       <c r="E42" t="n">
-        <v>353</v>
+        <v>51</v>
       </c>
       <c r="F42" t="n">
-        <v>0.2950143814086914</v>
+        <v>0.02498412132263184</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -1405,21 +1377,19 @@
       <c r="C43" t="n">
         <v>1</v>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D43" t="n">
+        <v>6</v>
       </c>
       <c r="E43" t="n">
-        <v>353</v>
+        <v>20</v>
       </c>
       <c r="F43" t="n">
-        <v>0.3400111198425293</v>
+        <v>0.01099753379821777</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1429,21 +1399,19 @@
       <c r="C44" t="n">
         <v>2</v>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D44" t="n">
+        <v>6</v>
       </c>
       <c r="E44" t="n">
-        <v>353</v>
+        <v>23</v>
       </c>
       <c r="F44" t="n">
-        <v>0.2859597206115723</v>
+        <v>0.01000857353210449</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -1453,21 +1421,19 @@
       <c r="C45" t="n">
         <v>3</v>
       </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D45" t="n">
+        <v>6</v>
       </c>
       <c r="E45" t="n">
-        <v>353</v>
+        <v>20</v>
       </c>
       <c r="F45" t="n">
-        <v>0.2379846572875977</v>
+        <v>0.01403331756591797</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -1477,216 +1443,14 @@
       <c r="C46" t="n">
         <v>4</v>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
+      <c r="D46" t="n">
+        <v>6</v>
       </c>
       <c r="E46" t="n">
-        <v>353</v>
+        <v>20</v>
       </c>
       <c r="F46" t="n">
-        <v>0.2559595108032227</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>46</v>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>UCS</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D47" t="n">
-        <v>32</v>
-      </c>
-      <c r="E47" t="n">
-        <v>774</v>
-      </c>
-      <c r="F47" t="n">
-        <v>0.8289790153503418</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>47</v>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>A*</t>
-        </is>
-      </c>
-      <c r="C48" t="n">
-        <v>1</v>
-      </c>
-      <c r="D48" t="n">
-        <v>32</v>
-      </c>
-      <c r="E48" t="n">
-        <v>605</v>
-      </c>
-      <c r="F48" t="n">
-        <v>0.5990183353424072</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>48</v>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>A*</t>
-        </is>
-      </c>
-      <c r="C49" t="n">
-        <v>2</v>
-      </c>
-      <c r="D49" t="n">
-        <v>32</v>
-      </c>
-      <c r="E49" t="n">
-        <v>629</v>
-      </c>
-      <c r="F49" t="n">
-        <v>0.5950002670288086</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>49</v>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>A*</t>
-        </is>
-      </c>
-      <c r="C50" t="n">
-        <v>3</v>
-      </c>
-      <c r="D50" t="n">
-        <v>32</v>
-      </c>
-      <c r="E50" t="n">
-        <v>566</v>
-      </c>
-      <c r="F50" t="n">
-        <v>0.5169796943664551</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>50</v>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>A*</t>
-        </is>
-      </c>
-      <c r="C51" t="n">
-        <v>4</v>
-      </c>
-      <c r="D51" t="n">
-        <v>32</v>
-      </c>
-      <c r="E51" t="n">
-        <v>583</v>
-      </c>
-      <c r="F51" t="n">
-        <v>0.5830404758453369</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>51</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>GBFS</t>
-        </is>
-      </c>
-      <c r="C52" t="n">
-        <v>1</v>
-      </c>
-      <c r="D52" t="n">
-        <v>42</v>
-      </c>
-      <c r="E52" t="n">
-        <v>315</v>
-      </c>
-      <c r="F52" t="n">
-        <v>0.260974645614624</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>52</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>GBFS</t>
-        </is>
-      </c>
-      <c r="C53" t="n">
-        <v>2</v>
-      </c>
-      <c r="D53" t="n">
-        <v>47</v>
-      </c>
-      <c r="E53" t="n">
-        <v>297</v>
-      </c>
-      <c r="F53" t="n">
-        <v>0.2889750003814697</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>53</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>GBFS</t>
-        </is>
-      </c>
-      <c r="C54" t="n">
-        <v>3</v>
-      </c>
-      <c r="D54" t="n">
-        <v>42</v>
-      </c>
-      <c r="E54" t="n">
-        <v>315</v>
-      </c>
-      <c r="F54" t="n">
-        <v>0.2529881000518799</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>54</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>GBFS</t>
-        </is>
-      </c>
-      <c r="C55" t="n">
-        <v>4</v>
-      </c>
-      <c r="D55" t="n">
-        <v>43</v>
-      </c>
-      <c r="E55" t="n">
-        <v>408</v>
-      </c>
-      <c r="F55" t="n">
-        <v>0.3879470825195312</v>
+        <v>0.01599526405334473</v>
       </c>
     </row>
   </sheetData>

</xml_diff>